<commit_message>
update weight and add pictures
</commit_message>
<xml_diff>
--- a/doc/daily_tracking.xlsx
+++ b/doc/daily_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\JJBaby\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E107058-E4A8-4E0D-ADBD-CFEF7D104F2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1875AB28-AE0C-44A1-ACFF-C1B9A8425D9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5A54F73C-E4A4-488F-8451-B849D94644A9}"/>
   </bookViews>
@@ -724,7 +724,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1645,11 +1645,21 @@
       <c r="F32" s="1">
         <v>57.2</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="G32" s="1">
+        <v>57.3</v>
+      </c>
+      <c r="H32" s="1">
+        <v>57.5</v>
+      </c>
+      <c r="I32" s="1">
+        <v>57.3</v>
+      </c>
+      <c r="J32" s="1">
+        <v>57.1</v>
+      </c>
+      <c r="K32" s="1">
+        <v>57.2</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
@@ -1659,15 +1669,17 @@
       <c r="B33" s="2">
         <v>30</v>
       </c>
-      <c r="C33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="7">
+        <v>57.5</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>

</xml_diff>